<commit_message>
Update MPNVbT to exclude electric motorbikes and natural gas freight HDVs
</commit_message>
<xml_diff>
--- a/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
+++ b/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="21" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="MPNVbT-motorbikes-psgr" sheetId="17" r:id="rId19"/>
     <sheet name="MPNVbT-motorbikes-frgt" sheetId="18" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2574,7 +2574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+    <sheetView topLeftCell="A77" workbookViewId="0">
       <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
@@ -4643,135 +4643,135 @@
       </c>
       <c r="E3" s="14">
         <f>Data!J23</f>
-        <v>9.9246334655016352E-2</v>
+        <v>9.793829616877181E-2</v>
       </c>
       <c r="F3" s="14">
         <f>Data!K23</f>
-        <v>9.9322181029181764E-2</v>
+        <v>9.7563274780050432E-2</v>
       </c>
       <c r="G3" s="14">
         <f>Data!L23</f>
-        <v>9.9423646431807233E-2</v>
+        <v>9.706158044570036E-2</v>
       </c>
       <c r="H3" s="14">
         <f>Data!M23</f>
-        <v>9.9558966796805551E-2</v>
+        <v>9.63924906999825E-2</v>
       </c>
       <c r="I3" s="14">
         <f>Data!N23</f>
-        <v>9.9738698562631345E-2</v>
+        <v>9.5503809373300497E-2</v>
       </c>
       <c r="J3" s="14">
         <f>Data!O23</f>
-        <v>9.9976119646789763E-2</v>
+        <v>9.4329883979073256E-2</v>
       </c>
       <c r="K3" s="14">
         <f>Data!P23</f>
-        <v>0.10028749869921928</v>
+        <v>9.2790274393963645E-2</v>
       </c>
       <c r="L3" s="14">
         <f>Data!Q23</f>
-        <v>0.10069204337913483</v>
+        <v>9.0790008602339642E-2</v>
       </c>
       <c r="M3" s="14">
         <f>Data!R23</f>
-        <v>0.10121124185307927</v>
+        <v>8.8222838650404409E-2</v>
       </c>
       <c r="N3" s="14">
         <f>Data!S23</f>
-        <v>0.10186723134327279</v>
+        <v>8.4979307337193458E-2</v>
       </c>
       <c r="O3" s="14">
         <f>Data!T23</f>
-        <v>0.10267984111843231</v>
+        <v>8.096136910715615E-2</v>
       </c>
       <c r="P3" s="14">
         <f>Data!U23</f>
-        <v>0.10366218964080433</v>
+        <v>7.610415989811814E-2</v>
       </c>
       <c r="Q3" s="14">
         <f>Data!V23</f>
-        <v>0.10481528538890343</v>
+        <v>7.0402693301471156E-2</v>
       </c>
       <c r="R3" s="14">
         <f>Data!W23</f>
-        <v>0.10612295260311078</v>
+        <v>6.3936950145602009E-2</v>
       </c>
       <c r="S3" s="14">
         <f>Data!X23</f>
-        <v>0.10754919519425249</v>
+        <v>5.6884912614880941E-2</v>
       </c>
       <c r="T3" s="14">
         <f>Data!Y23</f>
-        <v>0.10904010150526387</v>
+        <v>4.9513146180936024E-2</v>
       </c>
       <c r="U3" s="14">
         <f>Data!Z23</f>
-        <v>0.11053100781627526</v>
+        <v>4.2141379746991101E-2</v>
       </c>
       <c r="V3" s="14">
         <f>Data!AA23</f>
-        <v>0.11195725040741697</v>
+        <v>3.5089342216270039E-2</v>
       </c>
       <c r="W3" s="14">
         <f>Data!AB23</f>
-        <v>0.11326491762162431</v>
+        <v>2.8623599060400892E-2</v>
       </c>
       <c r="X3" s="14">
         <f>Data!AC23</f>
-        <v>0.11441801336972342</v>
+        <v>2.2922132463753908E-2</v>
       </c>
       <c r="Y3" s="14">
         <f>Data!AD23</f>
-        <v>0.11540036189209543</v>
+        <v>1.8064923254715898E-2</v>
       </c>
       <c r="Z3" s="14">
         <f>Data!AE23</f>
-        <v>0.11621297166725496</v>
+        <v>1.404698502467859E-2</v>
       </c>
       <c r="AA3" s="14">
         <f>Data!AF23</f>
-        <v>0.11686896115744848</v>
+        <v>1.0803453711467639E-2</v>
       </c>
       <c r="AB3" s="14">
         <f>Data!AG23</f>
-        <v>0.11738815963139292</v>
+        <v>8.2362837595324062E-3</v>
       </c>
       <c r="AC3" s="14">
         <f>Data!AH23</f>
-        <v>0.11779270431130845</v>
+        <v>6.2360179679084027E-3</v>
       </c>
       <c r="AD3" s="14">
         <f>Data!AI23</f>
-        <v>0.11810408336373798</v>
+        <v>4.6964083827987779E-3</v>
       </c>
       <c r="AE3" s="14">
         <f>Data!AJ23</f>
-        <v>0.1183415044478964</v>
+        <v>3.5224829885715514E-3</v>
       </c>
       <c r="AF3" s="14">
         <f>Data!AK23</f>
-        <v>0.11852123621372219</v>
+        <v>2.6338016618895621E-3</v>
       </c>
       <c r="AG3" s="14">
         <f>Data!AL23</f>
-        <v>0.11865655657872051</v>
+        <v>1.9647119161716742E-3</v>
       </c>
       <c r="AH3" s="14">
         <f>Data!AM23</f>
-        <v>0.11875802198134598</v>
+        <v>1.4630175818216157E-3</v>
       </c>
       <c r="AI3" s="14">
         <f>Data!AN23</f>
-        <v>0.11883386835551138</v>
+        <v>1.087996193100238E-3</v>
       </c>
       <c r="AJ3" s="14">
         <f>Data!AO23</f>
-        <v>0.1188904337893615</v>
+        <v>8.0830915743738962E-4</v>
       </c>
       <c r="AK3" s="14">
         <f>Data!AP23</f>
-        <v>0.11893254725748857</v>
+        <v>6.0007967416052244E-4</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.45">
@@ -5856,135 +5856,135 @@
       </c>
       <c r="E3" s="14">
         <f>Data!J30</f>
-        <v>7.9853890774704474E-3</v>
+        <v>6.677350591225901E-3</v>
       </c>
       <c r="F3" s="14">
         <f>Data!K30</f>
-        <v>8.4106881977561269E-3</v>
+        <v>6.6517819486247905E-3</v>
       </c>
       <c r="G3" s="14">
         <f>Data!L30</f>
-        <v>8.979642837327129E-3</v>
+        <v>6.6175768512202549E-3</v>
       </c>
       <c r="H3" s="14">
         <f>Data!M30</f>
-        <v>9.738434972400227E-3</v>
+        <v>6.5719588755771682E-3</v>
       </c>
       <c r="I3" s="14">
         <f>Data!N30</f>
-        <v>1.0746258520120493E-2</v>
+        <v>6.5113693307896452E-3</v>
       </c>
       <c r="J3" s="14">
         <f>Data!O30</f>
-        <v>1.2077567753303421E-2</v>
+        <v>6.4313320855869079E-3</v>
       </c>
       <c r="K3" s="14">
         <f>Data!P30</f>
-        <v>1.3823587105327589E-2</v>
+        <v>6.3263628000719456E-3</v>
       </c>
       <c r="L3" s="14">
         <f>Data!Q30</f>
-        <v>1.6092021138958794E-2</v>
+        <v>6.1899863621636018E-3</v>
       </c>
       <c r="M3" s="14">
         <f>Data!R30</f>
-        <v>1.9003362078483261E-2</v>
+        <v>6.0149588758083928E-3</v>
       </c>
       <c r="N3" s="14">
         <f>Data!S30</f>
-        <v>2.2681741647261729E-2</v>
+        <v>5.7938176411823951E-3</v>
       </c>
       <c r="O3" s="14">
         <f>Data!T30</f>
-        <v>2.7238350006116178E-2</v>
+        <v>5.5198779948400136E-3</v>
       </c>
       <c r="P3" s="14">
         <f>Data!U30</f>
-        <v>3.2746747302309039E-2</v>
+        <v>5.1887175596228505E-3</v>
       </c>
       <c r="Q3" s="14">
         <f>Data!V30</f>
-        <v>3.9212588453821674E-2</v>
+        <v>4.7999963663894066E-3</v>
       </c>
       <c r="R3" s="14">
         <f>Data!W30</f>
-        <v>4.6545169898202364E-2</v>
+        <v>4.3591674406935968E-3</v>
       </c>
       <c r="S3" s="14">
         <f>Data!X30</f>
-        <v>5.45426480374172E-2</v>
+        <v>3.8783654580456478E-3</v>
       </c>
       <c r="T3" s="14">
         <f>Data!Y30</f>
-        <v>6.2902719952242073E-2</v>
+        <v>3.37576462791423E-3</v>
       </c>
       <c r="U3" s="14">
         <f>Data!Z30</f>
-        <v>7.1262791867066966E-2</v>
+        <v>2.8731637977828122E-3</v>
       </c>
       <c r="V3" s="14">
         <f>Data!AA30</f>
-        <v>7.9260270006281788E-2</v>
+        <v>2.3923618151348632E-3</v>
       </c>
       <c r="W3" s="14">
         <f>Data!AB30</f>
-        <v>8.6592851450662478E-2</v>
+        <v>1.9515328894390534E-3</v>
       </c>
       <c r="X3" s="14">
         <f>Data!AC30</f>
-        <v>9.3058692602175114E-2</v>
+        <v>1.5628116962056095E-3</v>
       </c>
       <c r="Y3" s="14">
         <f>Data!AD30</f>
-        <v>9.8567089898367974E-2</v>
+        <v>1.2316512609884464E-3</v>
       </c>
       <c r="Z3" s="14">
         <f>Data!AE30</f>
-        <v>0.10312369825722244</v>
+        <v>9.5771161464606406E-4</v>
       </c>
       <c r="AA3" s="14">
         <f>Data!AF30</f>
-        <v>0.1068020778260009</v>
+        <v>7.3657038002006726E-4</v>
       </c>
       <c r="AB3" s="14">
         <f>Data!AG30</f>
-        <v>0.10971341876552537</v>
+        <v>5.615428936648582E-4</v>
       </c>
       <c r="AC3" s="14">
         <f>Data!AH30</f>
-        <v>0.11198185279915658</v>
+        <v>4.2516645575651352E-4</v>
       </c>
       <c r="AD3" s="14">
         <f>Data!AI30</f>
-        <v>0.11372787215118074</v>
+        <v>3.2019717024155212E-4</v>
       </c>
       <c r="AE3" s="14">
         <f>Data!AJ30</f>
-        <v>0.11505918138436366</v>
+        <v>2.4015992503881485E-4</v>
       </c>
       <c r="AF3" s="14">
         <f>Data!AK30</f>
-        <v>0.11606700493208393</v>
+        <v>1.7957038025129182E-4</v>
       </c>
       <c r="AG3" s="14">
         <f>Data!AL30</f>
-        <v>0.11682579706715704</v>
+        <v>1.3395240460820513E-4</v>
       </c>
       <c r="AH3" s="14">
         <f>Data!AM30</f>
-        <v>0.11739475170672803</v>
+        <v>9.9747307203669477E-5</v>
       </c>
       <c r="AI3" s="14">
         <f>Data!AN30</f>
-        <v>0.11782005082701372</v>
+        <v>7.4178664602558148E-5</v>
       </c>
       <c r="AJ3" s="14">
         <f>Data!AO30</f>
-        <v>0.11813723446986744</v>
+        <v>5.5109837943340817E-5</v>
       </c>
       <c r="AK3" s="14">
         <f>Data!AP30</f>
-        <v>0.11837338051038299</v>
+        <v>4.0912927054943815E-5</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.45">
@@ -14198,135 +14198,135 @@
       </c>
       <c r="E2" s="14">
         <f>Data!J78</f>
-        <v>1.098694263059318E-2</v>
+        <v>0</v>
       </c>
       <c r="F2" s="14">
         <f>Data!K78</f>
-        <v>1.4774031693273055E-2</v>
+        <v>0</v>
       </c>
       <c r="G2" s="14">
         <f>Data!L78</f>
-        <v>1.984030573407751E-2</v>
+        <v>0</v>
       </c>
       <c r="H2" s="14">
         <f>Data!M78</f>
-        <v>2.6596993576865863E-2</v>
+        <v>0</v>
       </c>
       <c r="I2" s="14">
         <f>Data!N78</f>
-        <v>3.5571189272636181E-2</v>
+        <v>0</v>
       </c>
       <c r="J2" s="14">
         <f>Data!O78</f>
-        <v>4.7425873177566781E-2</v>
+        <v>0</v>
       </c>
       <c r="K2" s="14">
         <f>Data!P78</f>
-        <v>6.2973356056996513E-2</v>
+        <v>0</v>
       </c>
       <c r="L2" s="14">
         <f>Data!Q78</f>
-        <v>8.317269649392238E-2</v>
+        <v>0</v>
       </c>
       <c r="M2" s="14">
         <f>Data!R78</f>
-        <v>0.10909682119561293</v>
+        <v>0</v>
       </c>
       <c r="N2" s="14">
         <f>Data!S78</f>
-        <v>0.14185106490048782</v>
+        <v>0</v>
       </c>
       <c r="O2" s="14">
         <f>Data!T78</f>
-        <v>0.18242552380635635</v>
+        <v>0</v>
       </c>
       <c r="P2" s="14">
         <f>Data!U78</f>
-        <v>0.23147521650098238</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="14">
         <f>Data!V78</f>
-        <v>0.28905049737499605</v>
+        <v>0</v>
       </c>
       <c r="R2" s="14">
         <f>Data!W78</f>
-        <v>0.35434369377420455</v>
+        <v>0</v>
       </c>
       <c r="S2" s="14">
         <f>Data!X78</f>
-        <v>0.42555748318834102</v>
+        <v>0</v>
       </c>
       <c r="T2" s="14">
         <f>Data!Y78</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="U2" s="14">
         <f>Data!Z78</f>
-        <v>0.57444251681165903</v>
+        <v>0</v>
       </c>
       <c r="V2" s="14">
         <f>Data!AA78</f>
-        <v>0.6456563062257954</v>
+        <v>0</v>
       </c>
       <c r="W2" s="14">
         <f>Data!AB78</f>
-        <v>0.71094950262500389</v>
+        <v>0</v>
       </c>
       <c r="X2" s="14">
         <f>Data!AC78</f>
-        <v>0.76852478349901754</v>
+        <v>0</v>
       </c>
       <c r="Y2" s="14">
         <f>Data!AD78</f>
-        <v>0.81757447619364365</v>
+        <v>0</v>
       </c>
       <c r="Z2" s="14">
         <f>Data!AE78</f>
-        <v>0.85814893509951229</v>
+        <v>0</v>
       </c>
       <c r="AA2" s="14">
         <f>Data!AF78</f>
-        <v>0.89090317880438707</v>
+        <v>0</v>
       </c>
       <c r="AB2" s="14">
         <f>Data!AG78</f>
-        <v>0.91682730350607766</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="14">
         <f>Data!AH78</f>
-        <v>0.9370266439430035</v>
+        <v>0</v>
       </c>
       <c r="AD2" s="14">
         <f>Data!AI78</f>
-        <v>0.95257412682243336</v>
+        <v>0</v>
       </c>
       <c r="AE2" s="14">
         <f>Data!AJ78</f>
-        <v>0.96442881072736386</v>
+        <v>0</v>
       </c>
       <c r="AF2" s="14">
         <f>Data!AK78</f>
-        <v>0.97340300642313404</v>
+        <v>0</v>
       </c>
       <c r="AG2" s="14">
         <f>Data!AL78</f>
-        <v>0.98015969426592253</v>
+        <v>0</v>
       </c>
       <c r="AH2" s="14">
         <f>Data!AM78</f>
-        <v>0.98522596830672693</v>
+        <v>0</v>
       </c>
       <c r="AI2" s="14">
         <f>Data!AN78</f>
-        <v>0.98901305736940681</v>
+        <v>0</v>
       </c>
       <c r="AJ2" s="14">
         <f>Data!AO78</f>
-        <v>0.99183742884684012</v>
+        <v>0</v>
       </c>
       <c r="AK2" s="14">
         <f>Data!AP78</f>
-        <v>0.99394019850841575</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.45">
@@ -55278,8 +55278,8 @@
   </sheetPr>
   <dimension ref="A1:AP91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -57845,7 +57845,7 @@
       </c>
       <c r="E23" s="41">
         <f>E30</f>
-        <v>0.1190539106486557</v>
+        <v>0</v>
       </c>
       <c r="F23" s="7" t="str">
         <f t="shared" si="1"/>
@@ -57858,135 +57858,135 @@
       </c>
       <c r="J23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:J$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,J$7))</f>
-        <v>9.9246334655016352E-2</v>
+        <v>9.793829616877181E-2</v>
       </c>
       <c r="K23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:K$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,K$7))</f>
-        <v>9.9322181029181764E-2</v>
+        <v>9.7563274780050432E-2</v>
       </c>
       <c r="L23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:L$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,L$7))</f>
-        <v>9.9423646431807233E-2</v>
+        <v>9.706158044570036E-2</v>
       </c>
       <c r="M23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:M$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,M$7))</f>
-        <v>9.9558966796805551E-2</v>
+        <v>9.63924906999825E-2</v>
       </c>
       <c r="N23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:N$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,N$7))</f>
-        <v>9.9738698562631345E-2</v>
+        <v>9.5503809373300497E-2</v>
       </c>
       <c r="O23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:O$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,O$7))</f>
-        <v>9.9976119646789763E-2</v>
+        <v>9.4329883979073256E-2</v>
       </c>
       <c r="P23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:P$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,P$7))</f>
-        <v>0.10028749869921928</v>
+        <v>9.2790274393963645E-2</v>
       </c>
       <c r="Q23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:Q$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,Q$7))</f>
-        <v>0.10069204337913483</v>
+        <v>9.0790008602339642E-2</v>
       </c>
       <c r="R23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:R$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,R$7))</f>
-        <v>0.10121124185307927</v>
+        <v>8.8222838650404409E-2</v>
       </c>
       <c r="S23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:S$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,S$7))</f>
-        <v>0.10186723134327279</v>
+        <v>8.4979307337193458E-2</v>
       </c>
       <c r="T23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:T$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,T$7))</f>
-        <v>0.10267984111843231</v>
+        <v>8.096136910715615E-2</v>
       </c>
       <c r="U23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:U$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,U$7))</f>
-        <v>0.10366218964080433</v>
+        <v>7.610415989811814E-2</v>
       </c>
       <c r="V23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:V$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,V$7))</f>
-        <v>0.10481528538890343</v>
+        <v>7.0402693301471156E-2</v>
       </c>
       <c r="W23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:W$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,W$7))</f>
-        <v>0.10612295260311078</v>
+        <v>6.3936950145602009E-2</v>
       </c>
       <c r="X23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:X$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,X$7))</f>
-        <v>0.10754919519425249</v>
+        <v>5.6884912614880941E-2</v>
       </c>
       <c r="Y23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:Y$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,Y$7))</f>
-        <v>0.10904010150526387</v>
+        <v>4.9513146180936024E-2</v>
       </c>
       <c r="Z23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:Z$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,Z$7))</f>
-        <v>0.11053100781627526</v>
+        <v>4.2141379746991101E-2</v>
       </c>
       <c r="AA23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AA$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AA$7))</f>
-        <v>0.11195725040741697</v>
+        <v>3.5089342216270039E-2</v>
       </c>
       <c r="AB23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AB$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AB$7))</f>
-        <v>0.11326491762162431</v>
+        <v>2.8623599060400892E-2</v>
       </c>
       <c r="AC23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AC$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AC$7))</f>
-        <v>0.11441801336972342</v>
+        <v>2.2922132463753908E-2</v>
       </c>
       <c r="AD23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AD$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AD$7))</f>
-        <v>0.11540036189209543</v>
+        <v>1.8064923254715898E-2</v>
       </c>
       <c r="AE23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AE$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AE$7))</f>
-        <v>0.11621297166725496</v>
+        <v>1.404698502467859E-2</v>
       </c>
       <c r="AF23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AF$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AF$7))</f>
-        <v>0.11686896115744848</v>
+        <v>1.0803453711467639E-2</v>
       </c>
       <c r="AG23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AG$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AG$7))</f>
-        <v>0.11738815963139292</v>
+        <v>8.2362837595324062E-3</v>
       </c>
       <c r="AH23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AH$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AH$7))</f>
-        <v>0.11779270431130845</v>
+        <v>6.2360179679084027E-3</v>
       </c>
       <c r="AI23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AI$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AI$7))</f>
-        <v>0.11810408336373798</v>
+        <v>4.6964083827987779E-3</v>
       </c>
       <c r="AJ23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AJ$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AJ$7))</f>
-        <v>0.1183415044478964</v>
+        <v>3.5224829885715514E-3</v>
       </c>
       <c r="AK23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AK$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AK$7))</f>
-        <v>0.11852123621372219</v>
+        <v>2.6338016618895621E-3</v>
       </c>
       <c r="AL23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AL$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AL$7))</f>
-        <v>0.11865655657872051</v>
+        <v>1.9647119161716742E-3</v>
       </c>
       <c r="AM23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AM$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AM$7))</f>
-        <v>0.11875802198134598</v>
+        <v>1.4630175818216157E-3</v>
       </c>
       <c r="AN23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AN$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AN$7))</f>
-        <v>0.11883386835551138</v>
+        <v>1.087996193100238E-3</v>
       </c>
       <c r="AO23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AO$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AO$7))</f>
-        <v>0.1188904337893615</v>
+        <v>8.0830915743738962E-4</v>
       </c>
       <c r="AP23" s="14">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$7:AP$7)+$I$4))),TREND($D23:$E23,$D$7:$E$7,AP$7))</f>
-        <v>0.11893254725748857</v>
+        <v>6.0007967416052244E-4</v>
       </c>
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.45">
@@ -58924,8 +58924,7 @@
         <v>6.75152925582846E-3</v>
       </c>
       <c r="E30" s="41">
-        <f>SUM(INDEX('AEO 50'!$214:$214,MATCH(E$7,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$225:$225,MATCH(E$7,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$236:$236,MATCH(E$7,'AEO 50'!$1:$1,0)))*Assumptions!A2/INDEX('AEO 50'!$243:$243,MATCH(E$7,'AEO 50'!$1:$1,0))</f>
-        <v>0.1190539106486557</v>
+        <v>0</v>
       </c>
       <c r="F30" s="7" t="str">
         <f t="shared" si="1"/>
@@ -58938,135 +58937,135 @@
       </c>
       <c r="J30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:J$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,J$7))</f>
-        <v>7.9853890774704474E-3</v>
+        <v>6.677350591225901E-3</v>
       </c>
       <c r="K30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:K$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,K$7))</f>
-        <v>8.4106881977561269E-3</v>
+        <v>6.6517819486247905E-3</v>
       </c>
       <c r="L30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:L$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,L$7))</f>
-        <v>8.979642837327129E-3</v>
+        <v>6.6175768512202549E-3</v>
       </c>
       <c r="M30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:M$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,M$7))</f>
-        <v>9.738434972400227E-3</v>
+        <v>6.5719588755771682E-3</v>
       </c>
       <c r="N30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:N$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,N$7))</f>
-        <v>1.0746258520120493E-2</v>
+        <v>6.5113693307896452E-3</v>
       </c>
       <c r="O30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:O$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,O$7))</f>
-        <v>1.2077567753303421E-2</v>
+        <v>6.4313320855869079E-3</v>
       </c>
       <c r="P30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:P$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,P$7))</f>
-        <v>1.3823587105327589E-2</v>
+        <v>6.3263628000719456E-3</v>
       </c>
       <c r="Q30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:Q$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,Q$7))</f>
-        <v>1.6092021138958794E-2</v>
+        <v>6.1899863621636018E-3</v>
       </c>
       <c r="R30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:R$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,R$7))</f>
-        <v>1.9003362078483261E-2</v>
+        <v>6.0149588758083928E-3</v>
       </c>
       <c r="S30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:S$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,S$7))</f>
-        <v>2.2681741647261729E-2</v>
+        <v>5.7938176411823951E-3</v>
       </c>
       <c r="T30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:T$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,T$7))</f>
-        <v>2.7238350006116178E-2</v>
+        <v>5.5198779948400136E-3</v>
       </c>
       <c r="U30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:U$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,U$7))</f>
-        <v>3.2746747302309039E-2</v>
+        <v>5.1887175596228505E-3</v>
       </c>
       <c r="V30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:V$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,V$7))</f>
-        <v>3.9212588453821674E-2</v>
+        <v>4.7999963663894066E-3</v>
       </c>
       <c r="W30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:W$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,W$7))</f>
-        <v>4.6545169898202364E-2</v>
+        <v>4.3591674406935968E-3</v>
       </c>
       <c r="X30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:X$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,X$7))</f>
-        <v>5.45426480374172E-2</v>
+        <v>3.8783654580456478E-3</v>
       </c>
       <c r="Y30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:Y$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,Y$7))</f>
-        <v>6.2902719952242073E-2</v>
+        <v>3.37576462791423E-3</v>
       </c>
       <c r="Z30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:Z$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,Z$7))</f>
-        <v>7.1262791867066966E-2</v>
+        <v>2.8731637977828122E-3</v>
       </c>
       <c r="AA30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AA$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AA$7))</f>
-        <v>7.9260270006281788E-2</v>
+        <v>2.3923618151348632E-3</v>
       </c>
       <c r="AB30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AB$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AB$7))</f>
-        <v>8.6592851450662478E-2</v>
+        <v>1.9515328894390534E-3</v>
       </c>
       <c r="AC30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AC$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AC$7))</f>
-        <v>9.3058692602175114E-2</v>
+        <v>1.5628116962056095E-3</v>
       </c>
       <c r="AD30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AD$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AD$7))</f>
-        <v>9.8567089898367974E-2</v>
+        <v>1.2316512609884464E-3</v>
       </c>
       <c r="AE30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AE$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AE$7))</f>
-        <v>0.10312369825722244</v>
+        <v>9.5771161464606406E-4</v>
       </c>
       <c r="AF30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AF$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AF$7))</f>
-        <v>0.1068020778260009</v>
+        <v>7.3657038002006726E-4</v>
       </c>
       <c r="AG30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AG$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AG$7))</f>
-        <v>0.10971341876552537</v>
+        <v>5.615428936648582E-4</v>
       </c>
       <c r="AH30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AH$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AH$7))</f>
-        <v>0.11198185279915658</v>
+        <v>4.2516645575651352E-4</v>
       </c>
       <c r="AI30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AI$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AI$7))</f>
-        <v>0.11372787215118074</v>
+        <v>3.2019717024155212E-4</v>
       </c>
       <c r="AJ30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AJ$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AJ$7))</f>
-        <v>0.11505918138436366</v>
+        <v>2.4015992503881485E-4</v>
       </c>
       <c r="AK30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AK$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AK$7))</f>
-        <v>0.11606700493208393</v>
+        <v>1.7957038025129182E-4</v>
       </c>
       <c r="AL30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AL$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AL$7))</f>
-        <v>0.11682579706715704</v>
+        <v>1.3395240460820513E-4</v>
       </c>
       <c r="AM30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AM$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AM$7))</f>
-        <v>0.11739475170672803</v>
+        <v>9.9747307203669477E-5</v>
       </c>
       <c r="AN30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AN$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AN$7))</f>
-        <v>0.11782005082701372</v>
+        <v>7.4178664602558148E-5</v>
       </c>
       <c r="AO30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AO$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AO$7))</f>
-        <v>0.11813723446986744</v>
+        <v>5.5109837943340817E-5</v>
       </c>
       <c r="AP30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AP$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AP$7))</f>
-        <v>0.11837338051038299</v>
+        <v>4.0912927054943815E-5</v>
       </c>
     </row>
     <row r="31" spans="1:42" x14ac:dyDescent="0.45">
@@ -66295,11 +66294,11 @@
         <v>0</v>
       </c>
       <c r="E78" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F78" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>s-curve</v>
+        <v>n/a</v>
       </c>
       <c r="H78" s="42"/>
       <c r="I78" s="41">
@@ -66308,135 +66307,135 @@
       </c>
       <c r="J78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:J$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,J$7))</f>
-        <v>1.098694263059318E-2</v>
+        <v>0</v>
       </c>
       <c r="K78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:K$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,K$7))</f>
-        <v>1.4774031693273055E-2</v>
+        <v>0</v>
       </c>
       <c r="L78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:L$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,L$7))</f>
-        <v>1.984030573407751E-2</v>
+        <v>0</v>
       </c>
       <c r="M78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:M$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,M$7))</f>
-        <v>2.6596993576865863E-2</v>
+        <v>0</v>
       </c>
       <c r="N78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:N$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,N$7))</f>
-        <v>3.5571189272636181E-2</v>
+        <v>0</v>
       </c>
       <c r="O78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:O$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,O$7))</f>
-        <v>4.7425873177566781E-2</v>
+        <v>0</v>
       </c>
       <c r="P78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:P$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,P$7))</f>
-        <v>6.2973356056996513E-2</v>
+        <v>0</v>
       </c>
       <c r="Q78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:Q$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,Q$7))</f>
-        <v>8.317269649392238E-2</v>
+        <v>0</v>
       </c>
       <c r="R78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:R$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,R$7))</f>
-        <v>0.10909682119561293</v>
+        <v>0</v>
       </c>
       <c r="S78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:S$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,S$7))</f>
-        <v>0.14185106490048782</v>
+        <v>0</v>
       </c>
       <c r="T78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:T$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,T$7))</f>
-        <v>0.18242552380635635</v>
+        <v>0</v>
       </c>
       <c r="U78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:U$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,U$7))</f>
-        <v>0.23147521650098238</v>
+        <v>0</v>
       </c>
       <c r="V78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:V$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,V$7))</f>
-        <v>0.28905049737499605</v>
+        <v>0</v>
       </c>
       <c r="W78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:W$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,W$7))</f>
-        <v>0.35434369377420455</v>
+        <v>0</v>
       </c>
       <c r="X78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:X$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,X$7))</f>
-        <v>0.42555748318834102</v>
+        <v>0</v>
       </c>
       <c r="Y78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:Y$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,Y$7))</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Z78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:Z$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,Z$7))</f>
-        <v>0.57444251681165903</v>
+        <v>0</v>
       </c>
       <c r="AA78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AA$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AA$7))</f>
-        <v>0.6456563062257954</v>
+        <v>0</v>
       </c>
       <c r="AB78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AB$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AB$7))</f>
-        <v>0.71094950262500389</v>
+        <v>0</v>
       </c>
       <c r="AC78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AC$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AC$7))</f>
-        <v>0.76852478349901754</v>
+        <v>0</v>
       </c>
       <c r="AD78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AD$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AD$7))</f>
-        <v>0.81757447619364365</v>
+        <v>0</v>
       </c>
       <c r="AE78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AE$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AE$7))</f>
-        <v>0.85814893509951229</v>
+        <v>0</v>
       </c>
       <c r="AF78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AF$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AF$7))</f>
-        <v>0.89090317880438707</v>
+        <v>0</v>
       </c>
       <c r="AG78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AG$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AG$7))</f>
-        <v>0.91682730350607766</v>
+        <v>0</v>
       </c>
       <c r="AH78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AH$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AH$7))</f>
-        <v>0.9370266439430035</v>
+        <v>0</v>
       </c>
       <c r="AI78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AI$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AI$7))</f>
-        <v>0.95257412682243336</v>
+        <v>0</v>
       </c>
       <c r="AJ78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AJ$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AJ$7))</f>
-        <v>0.96442881072736386</v>
+        <v>0</v>
       </c>
       <c r="AK78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AK$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AK$7))</f>
-        <v>0.97340300642313404</v>
+        <v>0</v>
       </c>
       <c r="AL78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AL$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AL$7))</f>
-        <v>0.98015969426592253</v>
+        <v>0</v>
       </c>
       <c r="AM78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AM$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AM$7))</f>
-        <v>0.98522596830672693</v>
+        <v>0</v>
       </c>
       <c r="AN78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AN$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AN$7))</f>
-        <v>0.98901305736940681</v>
+        <v>0</v>
       </c>
       <c r="AO78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AO$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AO$7))</f>
-        <v>0.99183742884684012</v>
+        <v>0</v>
       </c>
       <c r="AP78" s="14">
         <f>IF($F78="s-curve",$D78+($E78-$D78)*$I$2/(1+EXP($I$3*(COUNT($I$7:AP$7)+$I$4))),TREND($D78:$E78,$D$7:$E$7,AP$7))</f>
-        <v>0.99394019850841575</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:42" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
WRI edit to freight LDV MPNVbT
</commit_message>
<xml_diff>
--- a/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
+++ b/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-brazil\InputData\trans\MPNVbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-brazil\InputData\trans\MPNVbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="21" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="MPNVbT-motorbikes-psgr" sheetId="17" r:id="rId19"/>
     <sheet name="MPNVbT-motorbikes-frgt" sheetId="18" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2574,7 +2574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B125"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
       <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
@@ -3566,147 +3566,147 @@
       </c>
       <c r="B4" s="33">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="33">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="14">
         <f>Data!I17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="14">
         <f>Data!J17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="14">
         <f>Data!K17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="14">
         <f>Data!L17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="14">
         <f>Data!M17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="14">
         <f>Data!N17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="14">
         <f>Data!O17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="14">
         <f>Data!P17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="14">
         <f>Data!Q17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="14">
         <f>Data!R17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" s="14">
         <f>Data!S17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="14">
         <f>Data!T17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="14">
         <f>Data!U17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="14">
         <f>Data!V17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" s="14">
         <f>Data!W17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" s="14">
         <f>Data!X17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4" s="14">
         <f>Data!Y17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" s="14">
         <f>Data!Z17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" s="14">
         <f>Data!AA17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4" s="14">
         <f>Data!AB17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4" s="14">
         <f>Data!AC17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="14">
         <f>Data!AD17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="14">
         <f>Data!AE17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="14">
         <f>Data!AF17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="14">
         <f>Data!AG17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="14">
         <f>Data!AH17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="14">
         <f>Data!AI17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="14">
         <f>Data!AJ17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF4" s="14">
         <f>Data!AK17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4" s="14">
         <f>Data!AL17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="14">
         <f>Data!AM17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI4" s="14">
         <f>Data!AN17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ4" s="14">
         <f>Data!AO17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK4" s="14">
         <f>Data!AP17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.45">
@@ -55278,8 +55278,8 @@
   </sheetPr>
   <dimension ref="A1:AP91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -56909,10 +56909,10 @@
         <v>3</v>
       </c>
       <c r="D17" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="7" t="str">
         <f t="shared" si="1"/>
@@ -56921,139 +56921,139 @@
       <c r="H17" s="42"/>
       <c r="I17" s="41">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:J$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,J$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:K$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,K$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:L$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,L$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:M$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,M$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:N$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,N$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:O$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,O$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:P$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,P$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:Q$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,Q$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:R$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,R$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:S$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,S$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:T$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,T$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:U$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,U$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:V$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,V$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:W$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,W$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:X$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,X$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:Y$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,Y$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:Z$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,Z$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AA$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AA$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AB$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AB$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AC$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AC$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AD$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AD$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AE$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AE$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AF$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AF$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AG$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AG$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AH$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AH$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AI$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AI$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AJ$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AJ$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AK$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AK$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AL$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AL$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AM$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AM$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AN$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AN$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AO$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AO$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP17" s="14">
         <f>IF($F17="s-curve",$D17+($E17-$D17)*$I$2/(1+EXP($I$3*(COUNT($I$7:AP$7)+$I$4))),TREND($D17:$E17,$D$7:$E$7,AP$7))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Incorporate WRI edits for BNVP and MPNVbT
</commit_message>
<xml_diff>
--- a/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
+++ b/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" tabRatio="871"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="21" r:id="rId1"/>
@@ -33,22 +33,12 @@
     <sheet name="MPNVbT-motorbikes-psgr" sheetId="17" r:id="rId19"/>
     <sheet name="MPNVbT-motorbikes-frgt" sheetId="18" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="617">
   <si>
     <t>MPNVbT Max Percent New Vehicles by Technology</t>
   </si>
@@ -1888,6 +1878,18 @@
   <si>
     <t>Once the base year for Brazilian case is 2015, we added two columns for the years 2015 and 2016 and set the values for these years as the same as the 2017 values</t>
   </si>
+  <si>
+    <t xml:space="preserve">The exception are: </t>
+  </si>
+  <si>
+    <t>LDV-frgt. For Brazil, gasoline vehicles sales are set as zero. Once the vast majority of vehicles in Brazil is powered by diesel.</t>
+  </si>
+  <si>
+    <t>Med &amp; Heavy freight trucks powered by natural gas are set as zero. Once it is not expected the introduction of this technology.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDV-psgr, buses powered by gasoline and plug-in are set as zero also, following the same logic. </t>
+  </si>
 </sst>
 </file>
 
@@ -2572,10 +2574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B125"/>
+  <dimension ref="A1:B129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3085,6 +3087,26 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A126" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A127" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A128" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A129" t="s">
         <v>612</v>
       </c>
     </row>
@@ -3105,7 +3127,7 @@
   <dimension ref="A1:AK8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4319,7 +4341,7 @@
   <dimension ref="A1:AK8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4792,135 +4814,135 @@
       </c>
       <c r="E4" s="14">
         <f>Data!J24</f>
-        <v>6.117389182128008E-3</v>
+        <v>0</v>
       </c>
       <c r="F4" s="14">
         <f>Data!K24</f>
-        <v>1.2234778364256016E-2</v>
+        <v>0</v>
       </c>
       <c r="G4" s="14">
         <f>Data!L24</f>
-        <v>1.8352167546384024E-2</v>
+        <v>0</v>
       </c>
       <c r="H4" s="14">
         <f>Data!M24</f>
-        <v>2.4469556728512032E-2</v>
+        <v>0</v>
       </c>
       <c r="I4" s="14">
         <f>Data!N24</f>
-        <v>3.0586945910641816E-2</v>
+        <v>0</v>
       </c>
       <c r="J4" s="14">
         <f>Data!O24</f>
-        <v>3.6704335092769824E-2</v>
+        <v>0</v>
       </c>
       <c r="K4" s="14">
         <f>Data!P24</f>
-        <v>4.2821724274897832E-2</v>
+        <v>0</v>
       </c>
       <c r="L4" s="14">
         <f>Data!Q24</f>
-        <v>4.893911345702584E-2</v>
+        <v>0</v>
       </c>
       <c r="M4" s="14">
         <f>Data!R24</f>
-        <v>5.5056502639153848E-2</v>
+        <v>0</v>
       </c>
       <c r="N4" s="14">
         <f>Data!S24</f>
-        <v>6.1173891821281856E-2</v>
+        <v>0</v>
       </c>
       <c r="O4" s="14">
         <f>Data!T24</f>
-        <v>6.7291281003409864E-2</v>
+        <v>0</v>
       </c>
       <c r="P4" s="14">
         <f>Data!U24</f>
-        <v>7.3408670185537872E-2</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="14">
         <f>Data!V24</f>
-        <v>7.952605936766588E-2</v>
+        <v>0</v>
       </c>
       <c r="R4" s="14">
         <f>Data!W24</f>
-        <v>8.5643448549793888E-2</v>
+        <v>0</v>
       </c>
       <c r="S4" s="14">
         <f>Data!X24</f>
-        <v>9.1760837731921896E-2</v>
+        <v>0</v>
       </c>
       <c r="T4" s="14">
         <f>Data!Y24</f>
-        <v>9.787822691405168E-2</v>
+        <v>0</v>
       </c>
       <c r="U4" s="14">
         <f>Data!Z24</f>
-        <v>0.10399561609617969</v>
+        <v>0</v>
       </c>
       <c r="V4" s="14">
         <f>Data!AA24</f>
-        <v>0.1101130052783077</v>
+        <v>0</v>
       </c>
       <c r="W4" s="14">
         <f>Data!AB24</f>
-        <v>0.1162303944604357</v>
+        <v>0</v>
       </c>
       <c r="X4" s="14">
         <f>Data!AC24</f>
-        <v>0.12234778364256371</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="14">
         <f>Data!AD24</f>
-        <v>0.12846517282469172</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="14">
         <f>Data!AE24</f>
-        <v>0.13458256200681973</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="14">
         <f>Data!AF24</f>
-        <v>0.14069995118894774</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="14">
         <f>Data!AG24</f>
-        <v>0.14681734037107574</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="14">
         <f>Data!AH24</f>
-        <v>0.15293472955320375</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="14">
         <f>Data!AI24</f>
-        <v>0.15905211873533354</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="14">
         <f>Data!AJ24</f>
-        <v>0.16516950791746154</v>
+        <v>0</v>
       </c>
       <c r="AF4" s="14">
         <f>Data!AK24</f>
-        <v>0.17128689709958955</v>
+        <v>0</v>
       </c>
       <c r="AG4" s="14">
         <f>Data!AL24</f>
-        <v>0.17740428628171756</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="14">
         <f>Data!AM24</f>
-        <v>0.18352167546384557</v>
+        <v>0</v>
       </c>
       <c r="AI4" s="14">
         <f>Data!AN24</f>
-        <v>0.18963906464597358</v>
+        <v>0</v>
       </c>
       <c r="AJ4" s="14">
         <f>Data!AO24</f>
-        <v>0.19575645382810158</v>
+        <v>0</v>
       </c>
       <c r="AK4" s="14">
         <f>Data!AP24</f>
-        <v>0.20187384301022959</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.45">
@@ -5090,135 +5112,135 @@
       </c>
       <c r="E6" s="14">
         <f>Data!J26</f>
-        <v>4.2648579788926686E-4</v>
+        <v>0</v>
       </c>
       <c r="F6" s="14">
         <f>Data!K26</f>
-        <v>5.7349118008516366E-4</v>
+        <v>0</v>
       </c>
       <c r="G6" s="14">
         <f>Data!L26</f>
-        <v>7.7015134290440946E-4</v>
+        <v>0</v>
       </c>
       <c r="H6" s="14">
         <f>Data!M26</f>
-        <v>1.0324291669185613E-3</v>
+        <v>0</v>
       </c>
       <c r="I6" s="14">
         <f>Data!N26</f>
-        <v>1.3807851327600239E-3</v>
+        <v>0</v>
       </c>
       <c r="J6" s="14">
         <f>Data!O26</f>
-        <v>1.8409544895965047E-3</v>
+        <v>0</v>
       </c>
       <c r="K6" s="14">
         <f>Data!P26</f>
-        <v>2.4444691218236604E-3</v>
+        <v>0</v>
       </c>
       <c r="L6" s="14">
         <f>Data!Q26</f>
-        <v>3.2285572992836495E-3</v>
+        <v>0</v>
       </c>
       <c r="M6" s="14">
         <f>Data!R26</f>
-        <v>4.2348673693112402E-3</v>
+        <v>0</v>
       </c>
       <c r="N6" s="14">
         <f>Data!S26</f>
-        <v>5.5063056784397258E-3</v>
+        <v>0</v>
       </c>
       <c r="O6" s="14">
         <f>Data!T26</f>
-        <v>7.0813052995545534E-3</v>
+        <v>0</v>
       </c>
       <c r="P6" s="14">
         <f>Data!U26</f>
-        <v>8.985292425767618E-3</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="14">
         <f>Data!V26</f>
-        <v>1.1220221689335336E-2</v>
+        <v>0</v>
       </c>
       <c r="R6" s="14">
         <f>Data!W26</f>
-        <v>1.375474124580576E-2</v>
+        <v>0</v>
       </c>
       <c r="S6" s="14">
         <f>Data!X26</f>
-        <v>1.6519083503718002E-2</v>
+        <v>0</v>
       </c>
       <c r="T6" s="14">
         <f>Data!Y26</f>
-        <v>1.9408756932147605E-2</v>
+        <v>0</v>
       </c>
       <c r="U6" s="14">
         <f>Data!Z26</f>
-        <v>2.2298430360577208E-2</v>
+        <v>0</v>
       </c>
       <c r="V6" s="14">
         <f>Data!AA26</f>
-        <v>2.5062772618489448E-2</v>
+        <v>0</v>
       </c>
       <c r="W6" s="14">
         <f>Data!AB26</f>
-        <v>2.7597292174959872E-2</v>
+        <v>0</v>
       </c>
       <c r="X6" s="14">
         <f>Data!AC26</f>
-        <v>2.9832221438527588E-2</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="14">
         <f>Data!AD26</f>
-        <v>3.1736208564740652E-2</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="14">
         <f>Data!AE26</f>
-        <v>3.3311208185855486E-2</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="14">
         <f>Data!AF26</f>
-        <v>3.4582646494983972E-2</v>
+        <v>0</v>
       </c>
       <c r="AB6" s="14">
         <f>Data!AG26</f>
-        <v>3.5588956565011563E-2</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="14">
         <f>Data!AH26</f>
-        <v>3.637304474247155E-2</v>
+        <v>0</v>
       </c>
       <c r="AD6" s="14">
         <f>Data!AI26</f>
-        <v>3.6976559374698709E-2</v>
+        <v>0</v>
       </c>
       <c r="AE6" s="14">
         <f>Data!AJ26</f>
-        <v>3.7436728731535189E-2</v>
+        <v>0</v>
       </c>
       <c r="AF6" s="14">
         <f>Data!AK26</f>
-        <v>3.7785084697376646E-2</v>
+        <v>0</v>
       </c>
       <c r="AG6" s="14">
         <f>Data!AL26</f>
-        <v>3.80473625213908E-2</v>
+        <v>0</v>
       </c>
       <c r="AH6" s="14">
         <f>Data!AM26</f>
-        <v>3.8244022684210045E-2</v>
+        <v>0</v>
       </c>
       <c r="AI6" s="14">
         <f>Data!AN26</f>
-        <v>3.8391028066405944E-2</v>
+        <v>0</v>
       </c>
       <c r="AJ6" s="14">
         <f>Data!AO26</f>
-        <v>3.8500663145389129E-2</v>
+        <v>0</v>
       </c>
       <c r="AK6" s="14">
         <f>Data!AP26</f>
-        <v>3.8582287435880762E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.45">
@@ -5844,147 +5866,147 @@
       </c>
       <c r="B3" s="57">
         <f t="shared" ref="B3:B8" si="0">D3</f>
-        <v>6.75152925582846E-3</v>
+        <v>0</v>
       </c>
       <c r="C3" s="57">
         <f t="shared" ref="C3:C8" si="1">D3</f>
-        <v>6.75152925582846E-3</v>
+        <v>0</v>
       </c>
       <c r="D3" s="14">
         <f>Data!I30</f>
-        <v>6.75152925582846E-3</v>
+        <v>0</v>
       </c>
       <c r="E3" s="14">
         <f>Data!J30</f>
-        <v>6.677350591225901E-3</v>
+        <v>0</v>
       </c>
       <c r="F3" s="14">
         <f>Data!K30</f>
-        <v>6.6517819486247905E-3</v>
+        <v>0</v>
       </c>
       <c r="G3" s="14">
         <f>Data!L30</f>
-        <v>6.6175768512202549E-3</v>
+        <v>0</v>
       </c>
       <c r="H3" s="14">
         <f>Data!M30</f>
-        <v>6.5719588755771682E-3</v>
+        <v>0</v>
       </c>
       <c r="I3" s="14">
         <f>Data!N30</f>
-        <v>6.5113693307896452E-3</v>
+        <v>0</v>
       </c>
       <c r="J3" s="14">
         <f>Data!O30</f>
-        <v>6.4313320855869079E-3</v>
+        <v>0</v>
       </c>
       <c r="K3" s="14">
         <f>Data!P30</f>
-        <v>6.3263628000719456E-3</v>
+        <v>0</v>
       </c>
       <c r="L3" s="14">
         <f>Data!Q30</f>
-        <v>6.1899863621636018E-3</v>
+        <v>0</v>
       </c>
       <c r="M3" s="14">
         <f>Data!R30</f>
-        <v>6.0149588758083928E-3</v>
+        <v>0</v>
       </c>
       <c r="N3" s="14">
         <f>Data!S30</f>
-        <v>5.7938176411823951E-3</v>
+        <v>0</v>
       </c>
       <c r="O3" s="14">
         <f>Data!T30</f>
-        <v>5.5198779948400136E-3</v>
+        <v>0</v>
       </c>
       <c r="P3" s="14">
         <f>Data!U30</f>
-        <v>5.1887175596228505E-3</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="14">
         <f>Data!V30</f>
-        <v>4.7999963663894066E-3</v>
+        <v>0</v>
       </c>
       <c r="R3" s="14">
         <f>Data!W30</f>
-        <v>4.3591674406935968E-3</v>
+        <v>0</v>
       </c>
       <c r="S3" s="14">
         <f>Data!X30</f>
-        <v>3.8783654580456478E-3</v>
+        <v>0</v>
       </c>
       <c r="T3" s="14">
         <f>Data!Y30</f>
-        <v>3.37576462791423E-3</v>
+        <v>0</v>
       </c>
       <c r="U3" s="14">
         <f>Data!Z30</f>
-        <v>2.8731637977828122E-3</v>
+        <v>0</v>
       </c>
       <c r="V3" s="14">
         <f>Data!AA30</f>
-        <v>2.3923618151348632E-3</v>
+        <v>0</v>
       </c>
       <c r="W3" s="14">
         <f>Data!AB30</f>
-        <v>1.9515328894390534E-3</v>
+        <v>0</v>
       </c>
       <c r="X3" s="14">
         <f>Data!AC30</f>
-        <v>1.5628116962056095E-3</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="14">
         <f>Data!AD30</f>
-        <v>1.2316512609884464E-3</v>
+        <v>0</v>
       </c>
       <c r="Z3" s="14">
         <f>Data!AE30</f>
-        <v>9.5771161464606406E-4</v>
+        <v>0</v>
       </c>
       <c r="AA3" s="14">
         <f>Data!AF30</f>
-        <v>7.3657038002006726E-4</v>
+        <v>0</v>
       </c>
       <c r="AB3" s="14">
         <f>Data!AG30</f>
-        <v>5.615428936648582E-4</v>
+        <v>0</v>
       </c>
       <c r="AC3" s="14">
         <f>Data!AH30</f>
-        <v>4.2516645575651352E-4</v>
+        <v>0</v>
       </c>
       <c r="AD3" s="14">
         <f>Data!AI30</f>
-        <v>3.2019717024155212E-4</v>
+        <v>0</v>
       </c>
       <c r="AE3" s="14">
         <f>Data!AJ30</f>
-        <v>2.4015992503881485E-4</v>
+        <v>0</v>
       </c>
       <c r="AF3" s="14">
         <f>Data!AK30</f>
-        <v>1.7957038025129182E-4</v>
+        <v>0</v>
       </c>
       <c r="AG3" s="14">
         <f>Data!AL30</f>
-        <v>1.3395240460820513E-4</v>
+        <v>0</v>
       </c>
       <c r="AH3" s="14">
         <f>Data!AM30</f>
-        <v>9.9747307203669477E-5</v>
+        <v>0</v>
       </c>
       <c r="AI3" s="14">
         <f>Data!AN30</f>
-        <v>7.4178664602558148E-5</v>
+        <v>0</v>
       </c>
       <c r="AJ3" s="14">
         <f>Data!AO30</f>
-        <v>5.5109837943340817E-5</v>
+        <v>0</v>
       </c>
       <c r="AK3" s="14">
         <f>Data!AP30</f>
-        <v>4.0912927054943815E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.45">
@@ -5993,147 +6015,147 @@
       </c>
       <c r="B4" s="57">
         <f t="shared" si="0"/>
-        <v>0.16062618952794017</v>
+        <v>0</v>
       </c>
       <c r="C4" s="57">
         <f t="shared" si="1"/>
-        <v>0.16062618952794017</v>
+        <v>0</v>
       </c>
       <c r="D4" s="14">
         <f>Data!I31</f>
-        <v>0.16062618952794017</v>
+        <v>0</v>
       </c>
       <c r="E4" s="14">
         <f>Data!J31</f>
-        <v>0.16187611842134331</v>
+        <v>0</v>
       </c>
       <c r="F4" s="14">
         <f>Data!K31</f>
-        <v>0.163126047314746</v>
+        <v>0</v>
       </c>
       <c r="G4" s="14">
         <f>Data!L31</f>
-        <v>0.1643759762081487</v>
+        <v>0</v>
       </c>
       <c r="H4" s="14">
         <f>Data!M31</f>
-        <v>0.1656259051015514</v>
+        <v>0</v>
       </c>
       <c r="I4" s="14">
         <f>Data!N31</f>
-        <v>0.16687583399495409</v>
+        <v>0</v>
       </c>
       <c r="J4" s="14">
         <f>Data!O31</f>
-        <v>0.16812576288835679</v>
+        <v>0</v>
       </c>
       <c r="K4" s="14">
         <f>Data!P31</f>
-        <v>0.16937569178175949</v>
+        <v>0</v>
       </c>
       <c r="L4" s="14">
         <f>Data!Q31</f>
-        <v>0.17062562067516218</v>
+        <v>0</v>
       </c>
       <c r="M4" s="14">
         <f>Data!R31</f>
-        <v>0.17187554956856488</v>
+        <v>0</v>
       </c>
       <c r="N4" s="14">
         <f>Data!S31</f>
-        <v>0.17312547846196757</v>
+        <v>0</v>
       </c>
       <c r="O4" s="14">
         <f>Data!T31</f>
-        <v>0.17437540735537027</v>
+        <v>0</v>
       </c>
       <c r="P4" s="14">
         <f>Data!U31</f>
-        <v>0.17562533624877297</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="14">
         <f>Data!V31</f>
-        <v>0.17687526514217566</v>
+        <v>0</v>
       </c>
       <c r="R4" s="14">
         <f>Data!W31</f>
-        <v>0.17812519403557836</v>
+        <v>0</v>
       </c>
       <c r="S4" s="14">
         <f>Data!X31</f>
-        <v>0.17937512292898106</v>
+        <v>0</v>
       </c>
       <c r="T4" s="14">
         <f>Data!Y31</f>
-        <v>0.18062505182238375</v>
+        <v>0</v>
       </c>
       <c r="U4" s="14">
         <f>Data!Z31</f>
-        <v>0.18187498071578645</v>
+        <v>0</v>
       </c>
       <c r="V4" s="14">
         <f>Data!AA31</f>
-        <v>0.18312490960918915</v>
+        <v>0</v>
       </c>
       <c r="W4" s="14">
         <f>Data!AB31</f>
-        <v>0.18437483850259184</v>
+        <v>0</v>
       </c>
       <c r="X4" s="14">
         <f>Data!AC31</f>
-        <v>0.18562476739599454</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="14">
         <f>Data!AD31</f>
-        <v>0.18687469628939768</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="14">
         <f>Data!AE31</f>
-        <v>0.18812462518280038</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="14">
         <f>Data!AF31</f>
-        <v>0.18937455407620307</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="14">
         <f>Data!AG31</f>
-        <v>0.19062448296960577</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="14">
         <f>Data!AH31</f>
-        <v>0.19187441186300846</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="14">
         <f>Data!AI31</f>
-        <v>0.19312434075641116</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="14">
         <f>Data!AJ31</f>
-        <v>0.19437426964981386</v>
+        <v>0</v>
       </c>
       <c r="AF4" s="14">
         <f>Data!AK31</f>
-        <v>0.19562419854321655</v>
+        <v>0</v>
       </c>
       <c r="AG4" s="14">
         <f>Data!AL31</f>
-        <v>0.19687412743661925</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="14">
         <f>Data!AM31</f>
-        <v>0.19812405633002195</v>
+        <v>0</v>
       </c>
       <c r="AI4" s="14">
         <f>Data!AN31</f>
-        <v>0.19937398522342464</v>
+        <v>0</v>
       </c>
       <c r="AJ4" s="14">
         <f>Data!AO31</f>
-        <v>0.20062391411682734</v>
+        <v>0</v>
       </c>
       <c r="AK4" s="14">
         <f>Data!AP31</f>
-        <v>0.20187384301023004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.45">
@@ -55066,8 +55088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -55278,8 +55300,8 @@
   </sheetPr>
   <dimension ref="A1:AP91"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -57996,12 +58018,11 @@
         <v>0</v>
       </c>
       <c r="E24" s="41">
-        <f>E31</f>
-        <v>0.20187384301022987</v>
+        <v>0</v>
       </c>
       <c r="F24" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>linear</v>
+        <v>n/a</v>
       </c>
       <c r="H24" s="42"/>
       <c r="I24" s="41">
@@ -58010,135 +58031,135 @@
       </c>
       <c r="J24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:J$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,J$7))</f>
-        <v>6.117389182128008E-3</v>
+        <v>0</v>
       </c>
       <c r="K24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:K$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,K$7))</f>
-        <v>1.2234778364256016E-2</v>
+        <v>0</v>
       </c>
       <c r="L24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:L$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,L$7))</f>
-        <v>1.8352167546384024E-2</v>
+        <v>0</v>
       </c>
       <c r="M24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:M$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,M$7))</f>
-        <v>2.4469556728512032E-2</v>
+        <v>0</v>
       </c>
       <c r="N24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:N$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,N$7))</f>
-        <v>3.0586945910641816E-2</v>
+        <v>0</v>
       </c>
       <c r="O24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:O$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,O$7))</f>
-        <v>3.6704335092769824E-2</v>
+        <v>0</v>
       </c>
       <c r="P24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:P$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,P$7))</f>
-        <v>4.2821724274897832E-2</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:Q$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,Q$7))</f>
-        <v>4.893911345702584E-2</v>
+        <v>0</v>
       </c>
       <c r="R24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:R$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,R$7))</f>
-        <v>5.5056502639153848E-2</v>
+        <v>0</v>
       </c>
       <c r="S24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:S$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,S$7))</f>
-        <v>6.1173891821281856E-2</v>
+        <v>0</v>
       </c>
       <c r="T24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:T$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,T$7))</f>
-        <v>6.7291281003409864E-2</v>
+        <v>0</v>
       </c>
       <c r="U24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:U$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,U$7))</f>
-        <v>7.3408670185537872E-2</v>
+        <v>0</v>
       </c>
       <c r="V24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:V$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,V$7))</f>
-        <v>7.952605936766588E-2</v>
+        <v>0</v>
       </c>
       <c r="W24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:W$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,W$7))</f>
-        <v>8.5643448549793888E-2</v>
+        <v>0</v>
       </c>
       <c r="X24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:X$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,X$7))</f>
-        <v>9.1760837731921896E-2</v>
+        <v>0</v>
       </c>
       <c r="Y24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:Y$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,Y$7))</f>
-        <v>9.787822691405168E-2</v>
+        <v>0</v>
       </c>
       <c r="Z24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:Z$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,Z$7))</f>
-        <v>0.10399561609617969</v>
+        <v>0</v>
       </c>
       <c r="AA24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AA$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AA$7))</f>
-        <v>0.1101130052783077</v>
+        <v>0</v>
       </c>
       <c r="AB24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AB$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AB$7))</f>
-        <v>0.1162303944604357</v>
+        <v>0</v>
       </c>
       <c r="AC24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AC$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AC$7))</f>
-        <v>0.12234778364256371</v>
+        <v>0</v>
       </c>
       <c r="AD24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AD$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AD$7))</f>
-        <v>0.12846517282469172</v>
+        <v>0</v>
       </c>
       <c r="AE24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AE$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AE$7))</f>
-        <v>0.13458256200681973</v>
+        <v>0</v>
       </c>
       <c r="AF24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AF$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AF$7))</f>
-        <v>0.14069995118894774</v>
+        <v>0</v>
       </c>
       <c r="AG24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AG$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AG$7))</f>
-        <v>0.14681734037107574</v>
+        <v>0</v>
       </c>
       <c r="AH24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AH$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AH$7))</f>
-        <v>0.15293472955320375</v>
+        <v>0</v>
       </c>
       <c r="AI24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AI$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AI$7))</f>
-        <v>0.15905211873533354</v>
+        <v>0</v>
       </c>
       <c r="AJ24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AJ$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AJ$7))</f>
-        <v>0.16516950791746154</v>
+        <v>0</v>
       </c>
       <c r="AK24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AK$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AK$7))</f>
-        <v>0.17128689709958955</v>
+        <v>0</v>
       </c>
       <c r="AL24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AL$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AL$7))</f>
-        <v>0.17740428628171756</v>
+        <v>0</v>
       </c>
       <c r="AM24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AM$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AM$7))</f>
-        <v>0.18352167546384557</v>
+        <v>0</v>
       </c>
       <c r="AN24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AN$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AN$7))</f>
-        <v>0.18963906464597358</v>
+        <v>0</v>
       </c>
       <c r="AO24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AO$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AO$7))</f>
-        <v>0.19575645382810158</v>
+        <v>0</v>
       </c>
       <c r="AP24" s="14">
         <f>IF($F24="s-curve",$D24+($E24-$D24)*$I$2/(1+EXP($I$3*(COUNT($I$7:AP$7)+$I$4))),TREND($D24:$E24,$D$7:$E$7,AP$7))</f>
-        <v>0.20187384301022959</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:42" x14ac:dyDescent="0.45">
@@ -58302,12 +58323,11 @@
         <v>0</v>
       </c>
       <c r="E26" s="41">
-        <f>E33</f>
-        <v>3.881751386429521E-2</v>
+        <v>0</v>
       </c>
       <c r="F26" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>s-curve</v>
+        <v>n/a</v>
       </c>
       <c r="H26" s="42"/>
       <c r="I26" s="41">
@@ -58316,135 +58336,135 @@
       </c>
       <c r="J26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:J$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,J$7))</f>
-        <v>4.2648579788926686E-4</v>
+        <v>0</v>
       </c>
       <c r="K26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:K$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,K$7))</f>
-        <v>5.7349118008516366E-4</v>
+        <v>0</v>
       </c>
       <c r="L26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:L$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,L$7))</f>
-        <v>7.7015134290440946E-4</v>
+        <v>0</v>
       </c>
       <c r="M26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:M$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,M$7))</f>
-        <v>1.0324291669185613E-3</v>
+        <v>0</v>
       </c>
       <c r="N26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:N$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,N$7))</f>
-        <v>1.3807851327600239E-3</v>
+        <v>0</v>
       </c>
       <c r="O26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:O$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,O$7))</f>
-        <v>1.8409544895965047E-3</v>
+        <v>0</v>
       </c>
       <c r="P26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:P$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,P$7))</f>
-        <v>2.4444691218236604E-3</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:Q$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,Q$7))</f>
-        <v>3.2285572992836495E-3</v>
+        <v>0</v>
       </c>
       <c r="R26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:R$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,R$7))</f>
-        <v>4.2348673693112402E-3</v>
+        <v>0</v>
       </c>
       <c r="S26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:S$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,S$7))</f>
-        <v>5.5063056784397258E-3</v>
+        <v>0</v>
       </c>
       <c r="T26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:T$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,T$7))</f>
-        <v>7.0813052995545534E-3</v>
+        <v>0</v>
       </c>
       <c r="U26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:U$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,U$7))</f>
-        <v>8.985292425767618E-3</v>
+        <v>0</v>
       </c>
       <c r="V26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:V$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,V$7))</f>
-        <v>1.1220221689335336E-2</v>
+        <v>0</v>
       </c>
       <c r="W26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:W$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,W$7))</f>
-        <v>1.375474124580576E-2</v>
+        <v>0</v>
       </c>
       <c r="X26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:X$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,X$7))</f>
-        <v>1.6519083503718002E-2</v>
+        <v>0</v>
       </c>
       <c r="Y26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:Y$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,Y$7))</f>
-        <v>1.9408756932147605E-2</v>
+        <v>0</v>
       </c>
       <c r="Z26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:Z$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,Z$7))</f>
-        <v>2.2298430360577208E-2</v>
+        <v>0</v>
       </c>
       <c r="AA26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AA$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AA$7))</f>
-        <v>2.5062772618489448E-2</v>
+        <v>0</v>
       </c>
       <c r="AB26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AB$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AB$7))</f>
-        <v>2.7597292174959872E-2</v>
+        <v>0</v>
       </c>
       <c r="AC26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AC$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AC$7))</f>
-        <v>2.9832221438527588E-2</v>
+        <v>0</v>
       </c>
       <c r="AD26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AD$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AD$7))</f>
-        <v>3.1736208564740652E-2</v>
+        <v>0</v>
       </c>
       <c r="AE26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AE$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AE$7))</f>
-        <v>3.3311208185855486E-2</v>
+        <v>0</v>
       </c>
       <c r="AF26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AF$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AF$7))</f>
-        <v>3.4582646494983972E-2</v>
+        <v>0</v>
       </c>
       <c r="AG26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AG$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AG$7))</f>
-        <v>3.5588956565011563E-2</v>
+        <v>0</v>
       </c>
       <c r="AH26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AH$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AH$7))</f>
-        <v>3.637304474247155E-2</v>
+        <v>0</v>
       </c>
       <c r="AI26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AI$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AI$7))</f>
-        <v>3.6976559374698709E-2</v>
+        <v>0</v>
       </c>
       <c r="AJ26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AJ$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AJ$7))</f>
-        <v>3.7436728731535189E-2</v>
+        <v>0</v>
       </c>
       <c r="AK26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AK$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AK$7))</f>
-        <v>3.7785084697376646E-2</v>
+        <v>0</v>
       </c>
       <c r="AL26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AL$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AL$7))</f>
-        <v>3.80473625213908E-2</v>
+        <v>0</v>
       </c>
       <c r="AM26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AM$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AM$7))</f>
-        <v>3.8244022684210045E-2</v>
+        <v>0</v>
       </c>
       <c r="AN26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AN$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AN$7))</f>
-        <v>3.8391028066405944E-2</v>
+        <v>0</v>
       </c>
       <c r="AO26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AO$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AO$7))</f>
-        <v>3.8500663145389129E-2</v>
+        <v>0</v>
       </c>
       <c r="AP26" s="14">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($I$7:AP$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AP$7))</f>
-        <v>3.8582287435880762E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.45">
@@ -58918,152 +58938,151 @@
         <v>2</v>
       </c>
       <c r="D30" s="41">
-        <f>SUM(INDEX('AEO 50'!$214:$214,MATCH(D$7,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$225:$225,MATCH(D$7,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$236:$236,MATCH(D$7,'AEO 50'!$1:$1,0)))/INDEX('AEO 50'!$243:$243,MATCH(D$7,'AEO 50'!$1:$1,0))</f>
-        <v>6.75152925582846E-3</v>
+        <v>0</v>
       </c>
       <c r="E30" s="41">
         <v>0</v>
       </c>
       <c r="F30" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>s-curve</v>
+        <v>n/a</v>
       </c>
       <c r="H30" s="42"/>
       <c r="I30" s="41">
         <f t="shared" si="5"/>
-        <v>6.75152925582846E-3</v>
+        <v>0</v>
       </c>
       <c r="J30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:J$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,J$7))</f>
-        <v>6.677350591225901E-3</v>
+        <v>0</v>
       </c>
       <c r="K30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:K$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,K$7))</f>
-        <v>6.6517819486247905E-3</v>
+        <v>0</v>
       </c>
       <c r="L30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:L$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,L$7))</f>
-        <v>6.6175768512202549E-3</v>
+        <v>0</v>
       </c>
       <c r="M30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:M$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,M$7))</f>
-        <v>6.5719588755771682E-3</v>
+        <v>0</v>
       </c>
       <c r="N30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:N$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,N$7))</f>
-        <v>6.5113693307896452E-3</v>
+        <v>0</v>
       </c>
       <c r="O30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:O$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,O$7))</f>
-        <v>6.4313320855869079E-3</v>
+        <v>0</v>
       </c>
       <c r="P30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:P$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,P$7))</f>
-        <v>6.3263628000719456E-3</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:Q$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,Q$7))</f>
-        <v>6.1899863621636018E-3</v>
+        <v>0</v>
       </c>
       <c r="R30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:R$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,R$7))</f>
-        <v>6.0149588758083928E-3</v>
+        <v>0</v>
       </c>
       <c r="S30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:S$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,S$7))</f>
-        <v>5.7938176411823951E-3</v>
+        <v>0</v>
       </c>
       <c r="T30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:T$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,T$7))</f>
-        <v>5.5198779948400136E-3</v>
+        <v>0</v>
       </c>
       <c r="U30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:U$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,U$7))</f>
-        <v>5.1887175596228505E-3</v>
+        <v>0</v>
       </c>
       <c r="V30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:V$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,V$7))</f>
-        <v>4.7999963663894066E-3</v>
+        <v>0</v>
       </c>
       <c r="W30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:W$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,W$7))</f>
-        <v>4.3591674406935968E-3</v>
+        <v>0</v>
       </c>
       <c r="X30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:X$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,X$7))</f>
-        <v>3.8783654580456478E-3</v>
+        <v>0</v>
       </c>
       <c r="Y30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:Y$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,Y$7))</f>
-        <v>3.37576462791423E-3</v>
+        <v>0</v>
       </c>
       <c r="Z30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:Z$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,Z$7))</f>
-        <v>2.8731637977828122E-3</v>
+        <v>0</v>
       </c>
       <c r="AA30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AA$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AA$7))</f>
-        <v>2.3923618151348632E-3</v>
+        <v>0</v>
       </c>
       <c r="AB30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AB$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AB$7))</f>
-        <v>1.9515328894390534E-3</v>
+        <v>0</v>
       </c>
       <c r="AC30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AC$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AC$7))</f>
-        <v>1.5628116962056095E-3</v>
+        <v>0</v>
       </c>
       <c r="AD30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AD$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AD$7))</f>
-        <v>1.2316512609884464E-3</v>
+        <v>0</v>
       </c>
       <c r="AE30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AE$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AE$7))</f>
-        <v>9.5771161464606406E-4</v>
+        <v>0</v>
       </c>
       <c r="AF30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AF$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AF$7))</f>
-        <v>7.3657038002006726E-4</v>
+        <v>0</v>
       </c>
       <c r="AG30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AG$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AG$7))</f>
-        <v>5.615428936648582E-4</v>
+        <v>0</v>
       </c>
       <c r="AH30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AH$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AH$7))</f>
-        <v>4.2516645575651352E-4</v>
+        <v>0</v>
       </c>
       <c r="AI30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AI$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AI$7))</f>
-        <v>3.2019717024155212E-4</v>
+        <v>0</v>
       </c>
       <c r="AJ30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AJ$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AJ$7))</f>
-        <v>2.4015992503881485E-4</v>
+        <v>0</v>
       </c>
       <c r="AK30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AK$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AK$7))</f>
-        <v>1.7957038025129182E-4</v>
+        <v>0</v>
       </c>
       <c r="AL30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AL$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AL$7))</f>
-        <v>1.3395240460820513E-4</v>
+        <v>0</v>
       </c>
       <c r="AM30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AM$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AM$7))</f>
-        <v>9.9747307203669477E-5</v>
+        <v>0</v>
       </c>
       <c r="AN30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AN$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AN$7))</f>
-        <v>7.4178664602558148E-5</v>
+        <v>0</v>
       </c>
       <c r="AO30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AO$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AO$7))</f>
-        <v>5.5109837943340817E-5</v>
+        <v>0</v>
       </c>
       <c r="AP30" s="14">
         <f>IF($F30="s-curve",$D30+($E30-$D30)*$I$2/(1+EXP($I$3*(COUNT($I$7:AP$7)+$I$4))),TREND($D30:$E30,$D$7:$E$7,AP$7))</f>
-        <v>4.0912927054943815E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:42" x14ac:dyDescent="0.45">
@@ -59071,153 +59090,151 @@
         <v>3</v>
       </c>
       <c r="D31" s="41">
-        <f>SUM(INDEX('AEO 50'!$212:$212,MATCH(D$7,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$223:$223,MATCH(D$7,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$234:$234,MATCH(D$7,'AEO 50'!$1:$1,0)))/INDEX('AEO 50'!$243:$243,MATCH(D$7,'AEO 50'!$1:$1,0))</f>
-        <v>0.16062618952794017</v>
+        <v>0</v>
       </c>
       <c r="E31" s="41">
-        <f>SUM(INDEX('AEO 50'!$212:$212,MATCH(E$7,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$223:$223,MATCH(E$7,'AEO 50'!$1:$1,0)),INDEX('AEO 50'!$234:$234,MATCH(E$7,'AEO 50'!$1:$1,0)))/INDEX('AEO 50'!$243:$243,MATCH(E$7,'AEO 50'!$1:$1,0))</f>
-        <v>0.20187384301022987</v>
+        <v>0</v>
       </c>
       <c r="F31" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>linear</v>
+        <v>n/a</v>
       </c>
       <c r="H31" s="42"/>
       <c r="I31" s="41">
         <f t="shared" si="5"/>
-        <v>0.16062618952794017</v>
+        <v>0</v>
       </c>
       <c r="J31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:J$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,J$7))</f>
-        <v>0.16187611842134331</v>
+        <v>0</v>
       </c>
       <c r="K31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:K$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,K$7))</f>
-        <v>0.163126047314746</v>
+        <v>0</v>
       </c>
       <c r="L31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:L$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,L$7))</f>
-        <v>0.1643759762081487</v>
+        <v>0</v>
       </c>
       <c r="M31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:M$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,M$7))</f>
-        <v>0.1656259051015514</v>
+        <v>0</v>
       </c>
       <c r="N31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:N$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,N$7))</f>
-        <v>0.16687583399495409</v>
+        <v>0</v>
       </c>
       <c r="O31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:O$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,O$7))</f>
-        <v>0.16812576288835679</v>
+        <v>0</v>
       </c>
       <c r="P31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:P$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,P$7))</f>
-        <v>0.16937569178175949</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:Q$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,Q$7))</f>
-        <v>0.17062562067516218</v>
+        <v>0</v>
       </c>
       <c r="R31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:R$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,R$7))</f>
-        <v>0.17187554956856488</v>
+        <v>0</v>
       </c>
       <c r="S31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:S$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,S$7))</f>
-        <v>0.17312547846196757</v>
+        <v>0</v>
       </c>
       <c r="T31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:T$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,T$7))</f>
-        <v>0.17437540735537027</v>
+        <v>0</v>
       </c>
       <c r="U31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:U$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,U$7))</f>
-        <v>0.17562533624877297</v>
+        <v>0</v>
       </c>
       <c r="V31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:V$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,V$7))</f>
-        <v>0.17687526514217566</v>
+        <v>0</v>
       </c>
       <c r="W31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:W$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,W$7))</f>
-        <v>0.17812519403557836</v>
+        <v>0</v>
       </c>
       <c r="X31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:X$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,X$7))</f>
-        <v>0.17937512292898106</v>
+        <v>0</v>
       </c>
       <c r="Y31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:Y$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,Y$7))</f>
-        <v>0.18062505182238375</v>
+        <v>0</v>
       </c>
       <c r="Z31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:Z$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,Z$7))</f>
-        <v>0.18187498071578645</v>
+        <v>0</v>
       </c>
       <c r="AA31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AA$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AA$7))</f>
-        <v>0.18312490960918915</v>
+        <v>0</v>
       </c>
       <c r="AB31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AB$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AB$7))</f>
-        <v>0.18437483850259184</v>
+        <v>0</v>
       </c>
       <c r="AC31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AC$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AC$7))</f>
-        <v>0.18562476739599454</v>
+        <v>0</v>
       </c>
       <c r="AD31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AD$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AD$7))</f>
-        <v>0.18687469628939768</v>
+        <v>0</v>
       </c>
       <c r="AE31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AE$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AE$7))</f>
-        <v>0.18812462518280038</v>
+        <v>0</v>
       </c>
       <c r="AF31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AF$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AF$7))</f>
-        <v>0.18937455407620307</v>
+        <v>0</v>
       </c>
       <c r="AG31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AG$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AG$7))</f>
-        <v>0.19062448296960577</v>
+        <v>0</v>
       </c>
       <c r="AH31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AH$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AH$7))</f>
-        <v>0.19187441186300846</v>
+        <v>0</v>
       </c>
       <c r="AI31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AI$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AI$7))</f>
-        <v>0.19312434075641116</v>
+        <v>0</v>
       </c>
       <c r="AJ31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AJ$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AJ$7))</f>
-        <v>0.19437426964981386</v>
+        <v>0</v>
       </c>
       <c r="AK31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AK$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AK$7))</f>
-        <v>0.19562419854321655</v>
+        <v>0</v>
       </c>
       <c r="AL31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AL$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AL$7))</f>
-        <v>0.19687412743661925</v>
+        <v>0</v>
       </c>
       <c r="AM31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AM$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AM$7))</f>
-        <v>0.19812405633002195</v>
+        <v>0</v>
       </c>
       <c r="AN31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AN$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AN$7))</f>
-        <v>0.19937398522342464</v>
+        <v>0</v>
       </c>
       <c r="AO31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AO$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AO$7))</f>
-        <v>0.20062391411682734</v>
+        <v>0</v>
       </c>
       <c r="AP31" s="14">
         <f>IF($F31="s-curve",$D31+($E31-$D31)*$I$2/(1+EXP($I$3*(COUNT($I$7:AP$7)+$I$4))),TREND($D31:$E31,$D$7:$E$7,AP$7))</f>
-        <v>0.20187384301023004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:42" x14ac:dyDescent="0.45">

</xml_diff>